<commit_message>
Implemented a dual camera system with mobile checkout detection
</commit_message>
<xml_diff>
--- a/attendance_records/time_tracking_2025-10-09.xlsx
+++ b/attendance_records/time_tracking_2025-10-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="7" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
@@ -501,12 +501,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>darun</t>
+          <t>sajj</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1002</t>
+          <t>9876</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -515,10 +515,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="E2" t="n">
-        <v>2.1</v>
+        <v>3.8</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -530,153 +530,15 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>15:20:37</t>
+          <t>16:31:20</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>15:25:58</t>
+          <t>16:37:36</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>zayd</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Checked Out</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>15:22:53</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>15:23:57</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>sajj</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>9876</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Checked In</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>15:24:15</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>15:25:51</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>iyaaa</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1003</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Checked In</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>15:26:01</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>15:26:01</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
         <is>
           <t>2025-10-09</t>
         </is>
@@ -693,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -701,7 +563,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="7" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
@@ -756,12 +618,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>darun</t>
+          <t>sajj</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1002</t>
+          <t>9876</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -776,12 +638,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>15:20:37</t>
+          <t>16:31:20</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-10-09 15:20:37</t>
+          <t>2025-10-09 16:31:20</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -791,19 +653,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>attendance_records\check_in_darun_2025-10-09_15-20-37_1.jpg</t>
+          <t>attendance_records\check_in_sajj_2025-10-09_16-31-20_1.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>darun</t>
+          <t>sajj</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1002</t>
+          <t>9876</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -818,12 +680,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>15:21:42</t>
+          <t>16:32:26</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-10-09 15:21:42</t>
+          <t>2025-10-09 16:32:26</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -833,19 +695,19 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>attendance_records\check_out_darun_2025-10-09_15-21-42_2.jpg</t>
+          <t>attendance_records\check_out_sajj_2025-10-09_16-32-26_2.jpg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>darun</t>
+          <t>sajj</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1002</t>
+          <t>9876</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -860,12 +722,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>15:24:56</t>
+          <t>16:34:55</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-10-09 15:24:56</t>
+          <t>2025-10-09 16:34:55</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -875,19 +737,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>attendance_records\check_in_darun_2025-10-09_15-24-56_6.jpg</t>
+          <t>attendance_records\check_in_sajj_2025-10-09_16-34-55_3.jpg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>darun</t>
+          <t>sajj</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1002</t>
+          <t>9876</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -902,12 +764,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>15:25:58</t>
+          <t>16:37:36</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-10-09 15:25:58</t>
+          <t>2025-10-09 16:37:36</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -917,259 +779,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>attendance_records\check_out_darun_2025-10-09_15-25-58_9.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>zayd</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>CHECK_IN</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>15:22:53</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-10-09 15:22:53</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>attendance_records\check_in_zayd_2025-10-09_15-22-53_3.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>zayd</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>CHECK_OUT</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>15:23:57</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-10-09 15:23:57</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>attendance_records\check_out_zayd_2025-10-09_15-23-57_4.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>sajj</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>9876</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>CHECK_IN</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>15:24:15</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2025-10-09 15:24:15</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>attendance_records\check_in_sajj_2025-10-09_15-24-15_5.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>sajj</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>9876</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>CHECK_OUT</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>15:25:27</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2025-10-09 15:25:27</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>attendance_records\check_out_sajj_2025-10-09_15-25-27_7.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>sajj</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>9876</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>CHECK_IN</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>15:25:51</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2025-10-09 15:25:51</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>attendance_records\check_in_sajj_2025-10-09_15-25-51_8.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>iyaaa</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1003</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>AI&amp;DS</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>CHECK_IN</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>15:26:01</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2025-10-09 15:26:01</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2025-10-09</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>attendance_records\check_in_iyaaa_2025-10-09_15-26-01_10.jpg</t>
+          <t>attendance_records\check_out_sajj_2025-10-09_16-37-36_4.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>